<commit_message>
Just sent all the code files through the linter and cleaned up the documentation.
</commit_message>
<xml_diff>
--- a/clean_chrr-wphi/docs/dictionary.xlsx
+++ b/clean_chrr-wphi/docs/dictionary.xlsx
@@ -7,14 +7,13 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="813">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="751">
   <si>
     <t>variable</t>
   </si>
@@ -2517,192 +2516,6 @@
   <si>
     <t>year_structure_built</t>
   </si>
-  <si>
-    <t>time_trend_notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There is a moderate, (relatively) uniform, relative decline in values from 2012 to 2013. There is a large, uniform, relative decline in values from 2022 to 2023.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There is a large, uniform, relative decline in values from 2012 to 2013.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There is a large, (relatively) uniform, relative decline in values from 2012 to 2013. Additionally, there is a not a lot of variation in this variable.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moderate, (relatively) uniform, relative increase from 2017 to 2018. Large, uniform, relative increase from 2022 to 2023. Unrelated to the data provider recommended break points, there is a large, uniform, relative decrease from 2021 to 2022, and a very large, uniform, relative increase from 2014 to 2015..</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There is a very large, uniform, relative increase in values from 2010 to 2011. Values remain relatively static from 2011 to 2012.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There is only 1 data point available for this variable, and it stopped being updated in 2013.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There are only 3 data points available for this variable, and it stopped being updated in 2013.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moderate, (relatively) uniform, relative increase from 2021 to 2022.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Large, uniform, relative decline from 2015 to 2016. Large, uniform, relative increase from 2020 to 2021.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This variable only has three data points, and it has not been updated since 2012.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This variable has a lot of disjunctures so it is hard to say how comparable estimates across time really are.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This variable only has two data points and has not been updated since 2011.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There is only 1 data point available for this variable.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There is a large, uniform, relative increase from 2012 to 2013. From 2014 to 2015 and then 2015 to 2016, several states exhibit large variation (values which jump around quite a bit).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There are a few states which exhibit a large amount of variation otherwise there are no obvious disjunctures.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No discernible disjunctures between 2015 and 2016. Very large, uniform, relative decrease in values from 2020 to 2021.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There are only 2 data points available for this variable. A few states exhibit a relatively large amount of variation, but most states exhibit stable trends. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">There are only 2 data points available for this variable, and there are no obvious, discernible disjunctures.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There is only 1 data point available for this variable, and it stopped being updated in 2010.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There is a large, (relatively) uniform, relative increase in values from 2013 to 2014.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There are no obvious, discernible disjunctures.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A few states exhibit a great deal of variation while most states exhibit very little variation.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Large, uniform, relative decrease in values from 2021 to 2022.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There is a very large, uniform, relative decline from 2018 to 2019.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This variable only has three data points, and it has not been updated since 2015.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Because this variable is a binary variable, it is a bit harder to track progress over time.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There are only two data points available for this variable, and it was last updated in 2018.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No change from 2015 to 2016 (masks state-level variation), and large, (relatively) uniform, relative increase from 2020 to 2021. There are a few othe disjunctures in the data, but they do not appear major.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There are only 2 data points available for this variable, and it stopped being updated in 2013.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There appear to be no major disjunctures which would preclude an across-time comparison.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There is not much change in this variable when looking at national averages from 2020 to 2021. At the state level during this time period, there is a fair amount of heterogeneity.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moderate, uniform, increase in values from 2020 to 2021.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Large, uniform, relative increase from 2020 to 2021. Unrelated to the data provider recommended break points, there was a very large, uniform, relative decrease from 2022 to 2023.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There are only 2 data points available for this variable.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There is only one data point available for this variable, and it was last updated in 2010.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There are no major discernible disjunctures in the data. One state had a huge spike from 2011 to 2012 and achieved a 100% high school graduation rate fro 2012 to 2013 which is most likely a data error.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There is positive, linear growth in this variable at the national level (with a moderate amount of heterogeneity among states). Over time, though, the values are very stable. The only disjuncture comes in 2020 when values spike, but that was only for one state.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Several states exhibit a large amount of variation otherwise there are no obvious disjunctures.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There are only 2 data points available for this variable which exibhit no variation, and it stopped being updated in 2012.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There is very little variation in this variable across time.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There is a very large, uniform, relative increase in values from 2020 to 2021. Unrelated to the data provider recommended break points, there is a large, uniform, relative decline in values from 2022 to 2023.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unrelated to the data provider recommended break points, there is a very large, (relatively) uniform, decline in values from 2011 to 2012. Moderate, heterogeneous, increases in values from 2017 to 2018.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There are only 2 data points available for this variable. A few states exhibit a great deal of variation while most states exhibit very little variation. It stopped being updated in 2011.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In what is likely an error on the data provider's part, all values for this variable are missing.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unrelated to the data provider recommended break points, there is a large, uniform, relative decline from 2022 to 2023.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There are only 4 data points available for this variable and three out of the four data points exhibit no variation (they are the same value).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Very large, uniform, relative increase in values from 2013 to 2015.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There is a moderate, (relatively) uniform, relative decline in values from 2012 to 2013.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There are no major discernible disjunctures in the data.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Large, uniform, relative increase from 2021 to 2022. Unrelated to the data provider recommended break points, it appears as if there is a very large, uniform, relative decline from 2022 to 2023.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No change from 2015 to 2016 (masks state-level variation) and large, uniform, relative increase from 2020 to 2021.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slight relative decline from 2015 to 2016 (masks state-level variation) and large, uniform, relative increase from 2020 to 2021. Unrelated to the data provider recommended break points, there is a very large, uniform, relative decline from 2022 to 2023.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unrelated to the data provider recommended break points, there was a large, uniform, relative increase from 2021 to 2022.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Very large, uniform, relative decline from 2012 to 2013. Unrelated to the data provider recommended break points, there is a large, relative increase from 2011 to 2012. Many states did not have their value change during this time period, but a few did. I suspect the small number of states which did have their values increase are driving this observed nation-wide relative increase.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This variable only has one data point and has not been updated since 2010.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There is a moderate, uniform, relative increase in values from 2021 to 2022.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There is a moderate, heterogeneous, relative increase in values from 2021 to 2022.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unrelated to the data provider recommended break points, there was a large, (relatively) uniform, relative decline in values from 2019 to 2020.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Several states exhibit a great deal of variation for this variable. Otherwise, there are no discernible, obvious disjunctures.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unrelated to the data provider recommended break points, there is a large, uniform, relative increase from 2021 to 2022, and a large, uniform, relative decrease from 2022 to 2023.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There are no obvious, discernible disjunctures in the data. Many more states have data available starting in 2012. From 2019 to 2022, there is no variation in the value of this variable.</t>
-  </si>
 </sst>
 </file>
 
@@ -2749,7 +2562,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2763,14 +2576,8 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3279,7 +3086,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="N1" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A1" zoomScale="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
@@ -5583,7 +5390,7 @@
       </c>
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
-      <c r="N62" s="5" t="s">
+      <c r="N62" s="1" t="s">
         <v>273</v>
       </c>
       <c r="O62" s="1" t="s">
@@ -5596,7 +5403,7 @@
       <c r="A63" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B63" s="1" t="s">
         <v>275</v>
       </c>
       <c r="C63" s="1" t="s">
@@ -5621,16 +5428,16 @@
       <c r="J63" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="K63" s="5" t="s">
+      <c r="K63" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="N63" s="5" t="s">
+      <c r="N63" s="1" t="s">
         <v>281</v>
       </c>
       <c r="O63" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="P63" s="5" t="s">
+      <c r="P63" s="1" t="s">
         <v>282</v>
       </c>
     </row>
@@ -6306,7 +6113,7 @@
         <v>23</v>
       </c>
       <c r="L82" s="1"/>
-      <c r="N82" s="6" t="s">
+      <c r="N82" s="5" t="s">
         <v>343</v>
       </c>
       <c r="O82" s="1" t="s">
@@ -7663,7 +7470,7 @@
       <c r="J119" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K119" s="5" t="s">
+      <c r="K119" s="1" t="s">
         <v>499</v>
       </c>
       <c r="L119" s="1"/>
@@ -7707,7 +7514,7 @@
       <c r="J120" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K120" s="5" t="s">
+      <c r="K120" s="1" t="s">
         <v>506</v>
       </c>
       <c r="N120" s="1"/>
@@ -8794,16 +8601,16 @@
       </c>
     </row>
     <row r="150" ht="14.25">
-      <c r="A150" s="7" t="s">
+      <c r="A150" s="2" t="s">
         <v>611</v>
       </c>
-      <c r="B150" s="5" t="s">
+      <c r="B150" s="1" t="s">
         <v>612</v>
       </c>
-      <c r="C150" s="5" t="s">
+      <c r="C150" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D150" s="5" t="s">
+      <c r="D150" s="1" t="s">
         <v>251</v>
       </c>
       <c r="F150" s="1" t="s">
@@ -8825,14 +8632,14 @@
         <v>616</v>
       </c>
       <c r="L150" s="1"/>
-      <c r="O150" s="5" t="s">
+      <c r="O150" s="1" t="s">
         <v>24</v>
       </c>
       <c r="P150" s="1"/>
       <c r="R150" s="1"/>
     </row>
     <row r="151" ht="14.25">
-      <c r="A151" s="7" t="s">
+      <c r="A151" s="2" t="s">
         <v>617</v>
       </c>
       <c r="B151" s="1" t="s">
@@ -8856,17 +8663,17 @@
       <c r="I151" s="1">
         <v>1</v>
       </c>
-      <c r="J151" s="5" t="s">
+      <c r="J151" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="K151" s="5" t="s">
+      <c r="K151" s="1" t="s">
         <v>616</v>
       </c>
       <c r="L151" s="1"/>
       <c r="N151" s="1" t="s">
         <v>619</v>
       </c>
-      <c r="O151" s="5" t="s">
+      <c r="O151" s="1" t="s">
         <v>24</v>
       </c>
       <c r="P151" s="1"/>
@@ -9911,584 +9718,4 @@
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
-  <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <sheetData>
-    <row r="1" ht="14.25">
-      <c r="A1" s="3" t="s">
-        <v>751</v>
-      </c>
-    </row>
-    <row r="2" ht="14.25">
-      <c r="A2" s="1"/>
-    </row>
-    <row r="3" ht="14.25">
-      <c r="A3" s="1"/>
-    </row>
-    <row r="4" ht="14.25">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" ht="14.25">
-      <c r="A5" s="1"/>
-    </row>
-    <row r="6" ht="285">
-      <c r="A6" s="1" t="s">
-        <v>752</v>
-      </c>
-    </row>
-    <row r="7" ht="14.25">
-      <c r="A7" s="1"/>
-    </row>
-    <row r="8" ht="14.25">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" ht="14.25">
-      <c r="A9" s="1"/>
-    </row>
-    <row r="10" ht="14.25">
-      <c r="A10" s="1"/>
-    </row>
-    <row r="11" ht="128.25">
-      <c r="A11" s="1" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="12" ht="242.25">
-      <c r="A12" s="1" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="13" ht="409.5">
-      <c r="A13" s="1" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="14" ht="242.25">
-      <c r="A14" s="1" t="s">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="15" ht="171">
-      <c r="A15" s="1" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="16" ht="171">
-      <c r="A16" s="1" t="s">
-        <v>758</v>
-      </c>
-    </row>
-    <row r="17" ht="14.25">
-      <c r="A17" s="1"/>
-    </row>
-    <row r="18" ht="14.25">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="19" ht="14.25">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" ht="128.25">
-      <c r="A20" s="1" t="s">
-        <v>759</v>
-      </c>
-    </row>
-    <row r="21" ht="199.5">
-      <c r="A21" s="1" t="s">
-        <v>760</v>
-      </c>
-    </row>
-    <row r="22" ht="14.25">
-      <c r="A22" s="1"/>
-    </row>
-    <row r="23" ht="14.25">
-      <c r="A23" s="1"/>
-    </row>
-    <row r="24" ht="156.75">
-      <c r="A24" s="1" t="s">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="25" ht="156.75">
-      <c r="A25" s="1" t="s">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="26" ht="199.5">
-      <c r="A26" s="1" t="s">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="28" ht="14.25">
-      <c r="A28" s="1"/>
-    </row>
-    <row r="29" ht="142.5">
-      <c r="A29" s="1" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="31" ht="14.25">
-      <c r="A31" s="1"/>
-    </row>
-    <row r="32" ht="14.25">
-      <c r="A32" s="1"/>
-    </row>
-    <row r="33" ht="14.25">
-      <c r="A33" s="1"/>
-    </row>
-    <row r="34" ht="99.75">
-      <c r="A34" s="1" t="s">
-        <v>764</v>
-      </c>
-    </row>
-    <row r="36" ht="14.25">
-      <c r="A36" s="1"/>
-    </row>
-    <row r="37" ht="14.25">
-      <c r="A37" s="1"/>
-    </row>
-    <row r="38" ht="342">
-      <c r="A38" s="1" t="s">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="39" ht="213.75">
-      <c r="A39" s="1" t="s">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="40" ht="14.25">
-      <c r="A40" s="1"/>
-    </row>
-    <row r="41" ht="242.25">
-      <c r="A41" s="1" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="43" ht="285">
-      <c r="A43" s="1" t="s">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="44" ht="199.5">
-      <c r="A44" s="1" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="47" ht="171">
-      <c r="A47" s="1" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="48" ht="14.25">
-      <c r="A48" s="1"/>
-    </row>
-    <row r="50" ht="14.25">
-      <c r="A50" s="1"/>
-    </row>
-    <row r="51" ht="14.25">
-      <c r="A51" s="1"/>
-    </row>
-    <row r="52" ht="142.5">
-      <c r="A52" s="1" t="s">
-        <v>771</v>
-      </c>
-    </row>
-    <row r="53" ht="99.75">
-      <c r="A53" s="1" t="s">
-        <v>764</v>
-      </c>
-    </row>
-    <row r="54" ht="99.75">
-      <c r="A54" s="1" t="s">
-        <v>772</v>
-      </c>
-    </row>
-    <row r="55" ht="14.25">
-      <c r="A55" s="1"/>
-    </row>
-    <row r="56" ht="14.25">
-      <c r="A56" s="1"/>
-    </row>
-    <row r="57" ht="14.25">
-      <c r="A57" s="1"/>
-    </row>
-    <row r="58" ht="171">
-      <c r="A58" s="1" t="s">
-        <v>773</v>
-      </c>
-    </row>
-    <row r="59" ht="114">
-      <c r="A59" s="1" t="s">
-        <v>774</v>
-      </c>
-    </row>
-    <row r="61" ht="128.25">
-      <c r="A61" s="1" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="62" ht="156.75">
-      <c r="A62" s="1" t="s">
-        <v>776</v>
-      </c>
-    </row>
-    <row r="63" ht="156.75">
-      <c r="A63" s="1" t="s">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="64" ht="14.25">
-      <c r="A64" s="1"/>
-    </row>
-    <row r="65" ht="14.25">
-      <c r="A65" s="1"/>
-    </row>
-    <row r="66" ht="14.25">
-      <c r="A66" s="1"/>
-    </row>
-    <row r="67" ht="14.25">
-      <c r="A67" s="1" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="68" ht="14.25">
-      <c r="A68" s="1"/>
-    </row>
-    <row r="69" ht="14.25">
-      <c r="A69" s="1" t="s">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="71" ht="14.25">
-      <c r="A71" s="1"/>
-    </row>
-    <row r="72" ht="14.25">
-      <c r="A72" s="1"/>
-    </row>
-    <row r="73" ht="14.25">
-      <c r="A73" s="1"/>
-    </row>
-    <row r="74" ht="14.25">
-      <c r="A74" s="1" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="75" ht="14.25">
-      <c r="A75" s="1"/>
-    </row>
-    <row r="76" ht="14.25">
-      <c r="A76" s="1"/>
-    </row>
-    <row r="77" ht="14.25">
-      <c r="A77" s="1"/>
-    </row>
-    <row r="78" ht="14.25">
-      <c r="A78" s="1"/>
-    </row>
-    <row r="80" ht="14.25">
-      <c r="A80" s="1"/>
-    </row>
-    <row r="81" ht="14.25">
-      <c r="A81" s="1" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="82" ht="14.25">
-      <c r="A82" s="1" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="83" ht="14.25">
-      <c r="A83" s="1" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="84" ht="14.25">
-      <c r="A84" s="1" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="85" ht="14.25">
-      <c r="A85" s="1"/>
-    </row>
-    <row r="86" ht="14.25">
-      <c r="A86" s="1" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="87" ht="14.25">
-      <c r="A87" s="1" t="s">
-        <v>786</v>
-      </c>
-    </row>
-    <row r="88" ht="14.25">
-      <c r="A88" s="1"/>
-    </row>
-    <row r="89" ht="14.25">
-      <c r="A89" s="1"/>
-    </row>
-    <row r="90" ht="14.25">
-      <c r="A90" s="1" t="s">
-        <v>772</v>
-      </c>
-    </row>
-    <row r="91" ht="14.25">
-      <c r="A91" s="1"/>
-    </row>
-    <row r="92" ht="14.25">
-      <c r="A92" s="1" t="s">
-        <v>787</v>
-      </c>
-    </row>
-    <row r="93" ht="14.25">
-      <c r="A93" s="1" t="s">
-        <v>788</v>
-      </c>
-    </row>
-    <row r="95" ht="14.25">
-      <c r="A95" s="1" t="s">
-        <v>789</v>
-      </c>
-    </row>
-    <row r="96" ht="14.25">
-      <c r="A96" s="1" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="97" ht="14.25">
-      <c r="A97" s="1" t="s">
-        <v>790</v>
-      </c>
-    </row>
-    <row r="98" ht="14.25">
-      <c r="A98" s="1" t="s">
-        <v>791</v>
-      </c>
-    </row>
-    <row r="100" ht="14.25">
-      <c r="A100" s="1"/>
-    </row>
-    <row r="101" ht="14.25">
-      <c r="A101" s="1"/>
-    </row>
-    <row r="102" ht="14.25">
-      <c r="A102" s="1"/>
-    </row>
-    <row r="103" ht="14.25">
-      <c r="A103" s="1"/>
-    </row>
-    <row r="104" ht="14.25">
-      <c r="A104" s="1" t="s">
-        <v>792</v>
-      </c>
-    </row>
-    <row r="105" ht="14.25">
-      <c r="A105" s="1"/>
-    </row>
-    <row r="106" ht="14.25">
-      <c r="A106" s="1" t="s">
-        <v>772</v>
-      </c>
-    </row>
-    <row r="107" ht="14.25">
-      <c r="A107" s="1"/>
-    </row>
-    <row r="108" ht="14.25">
-      <c r="A108" s="1"/>
-    </row>
-    <row r="109" ht="14.25">
-      <c r="A109" s="1" t="s">
-        <v>793</v>
-      </c>
-    </row>
-    <row r="110" ht="14.25">
-      <c r="A110" s="1" t="s">
-        <v>794</v>
-      </c>
-    </row>
-    <row r="111" ht="14.25">
-      <c r="A111" s="1" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="112" ht="14.25">
-      <c r="A112" s="1"/>
-    </row>
-    <row r="113" ht="14.25">
-      <c r="A113" s="1"/>
-    </row>
-    <row r="114" ht="14.25">
-      <c r="A114" s="1"/>
-    </row>
-    <row r="115" ht="14.25">
-      <c r="A115" s="1"/>
-    </row>
-    <row r="116" ht="14.25">
-      <c r="A116" s="1"/>
-    </row>
-    <row r="117" ht="14.25">
-      <c r="A117" s="1"/>
-    </row>
-    <row r="118" ht="14.25">
-      <c r="A118" s="1"/>
-    </row>
-    <row r="119" ht="14.25">
-      <c r="A119" s="1" t="s">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="121" ht="14.25">
-      <c r="A121" s="1" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="123" ht="14.25">
-      <c r="A123" s="1" t="s">
-        <v>798</v>
-      </c>
-    </row>
-    <row r="124" ht="14.25">
-      <c r="A124" s="1" t="s">
-        <v>799</v>
-      </c>
-    </row>
-    <row r="129" ht="14.25">
-      <c r="A129" s="1" t="s">
-        <v>772</v>
-      </c>
-    </row>
-    <row r="130" ht="14.25">
-      <c r="A130" s="1" t="s">
-        <v>772</v>
-      </c>
-    </row>
-    <row r="136" ht="14.25">
-      <c r="A136" s="1" t="s">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="141" ht="14.25">
-      <c r="A141" s="1" t="s">
-        <v>801</v>
-      </c>
-    </row>
-    <row r="142" ht="14.25">
-      <c r="A142" s="1" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="143" ht="14.25">
-      <c r="A143" s="1" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="144" ht="14.25">
-      <c r="A144" s="1" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="148" ht="14.25">
-      <c r="A148" s="1" t="s">
-        <v>804</v>
-      </c>
-    </row>
-    <row r="149" ht="14.25">
-      <c r="A149" s="1"/>
-    </row>
-    <row r="150" ht="14.25">
-      <c r="A150" s="1"/>
-    </row>
-    <row r="151" ht="14.25">
-      <c r="A151" s="1"/>
-    </row>
-    <row r="152" ht="14.25">
-      <c r="A152" s="1" t="s">
-        <v>805</v>
-      </c>
-    </row>
-    <row r="153" ht="14.25">
-      <c r="A153" s="1" t="s">
-        <v>806</v>
-      </c>
-    </row>
-    <row r="155" ht="14.25">
-      <c r="A155" s="1" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="156" ht="14.25">
-      <c r="A156" s="1" t="s">
-        <v>807</v>
-      </c>
-    </row>
-    <row r="157" ht="14.25">
-      <c r="A157" s="1" t="s">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="158" ht="14.25">
-      <c r="A158" s="1" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="159" ht="14.25">
-      <c r="A159" s="1" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="161" ht="14.25">
-      <c r="A161" s="1" t="s">
-        <v>772</v>
-      </c>
-    </row>
-    <row r="164" ht="14.25">
-      <c r="A164" s="1" t="s">
-        <v>786</v>
-      </c>
-    </row>
-    <row r="166" ht="14.25">
-      <c r="A166" s="1" t="s">
-        <v>809</v>
-      </c>
-    </row>
-    <row r="169" ht="14.25">
-      <c r="A169" s="1"/>
-    </row>
-    <row r="172" ht="14.25">
-      <c r="A172" s="1" t="s">
-        <v>810</v>
-      </c>
-    </row>
-    <row r="173" ht="14.25">
-      <c r="A173" s="1" t="s">
-        <v>811</v>
-      </c>
-    </row>
-    <row r="174" ht="14.25">
-      <c r="A174" s="1"/>
-    </row>
-    <row r="177" ht="14.25">
-      <c r="A177" s="1" t="s">
-        <v>812</v>
-      </c>
-    </row>
-    <row r="178" ht="14.25">
-      <c r="A178" s="1" t="s">
-        <v>764</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
-  <headerFooter/>
-</worksheet>
 </file>
</xml_diff>